<commit_message>
update excel of download well
</commit_message>
<xml_diff>
--- a/static/download_template/monitoring_data.xlsx
+++ b/static/download_template/monitoring_data.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Level Measurement" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Quality Measurement" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Yield Measurement" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Groundwater Level" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Groundwater Quality" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Abstraction-Discharge" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -39,13 +39,13 @@
     <t xml:space="preserve">Unit</t>
   </si>
   <si>
-    <t xml:space="preserve">Method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The original ID of the groundwater point.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The date and time of the measurement or sampling (yyyy-mm-dd hh:MM)</t>
+    <t xml:space="preserve">Methodology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As recorded in the original database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The date and time of the measurement or sampling (yyyy-mm-dd hh:MM:ss).</t>
   </si>
   <si>
     <t xml:space="preserve">One of the following:
@@ -54,7 +54,7 @@
 • Water level elevation a.m.s.l.</t>
   </si>
   <si>
-    <t xml:space="preserve">Value (number)</t>
+    <t xml:space="preserve">The numeric value of the measurement.</t>
   </si>
   <si>
     <t xml:space="preserve">Unit must be either: 
@@ -65,16 +65,82 @@
     <t xml:space="preserve">Explain the methodology used to collect the data, in the field and eventually in the lab.</t>
   </si>
   <si>
+    <t xml:space="preserve">The date and time of the measurement or sampling (yyyy-mm-dd hh:MM:ss)</t>
+  </si>
+  <si>
     <t xml:space="preserve">One of the following:
-• EC, pH, T, NO3, Cl, Ca, Mg, Na, K, HCO3, SO4, TDS, FC, FS, E Coli, F, As, U, NH4, Fe, Mn, P</t>
+• EC
+• pH
+• T
+• NO3
+• Cl
+• Ca
+• Mg
+• Na
+• K
+• HCO3
+• SO4
+• TDS
+• FC
+• FS
+• E Coli
+• F
+• As
+• U
+• NH4
+• Fe
+• Mn
+• P</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">One of the following:
+• (blank)
+• S/m
+• μS/cm
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">°</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">C
+• °F
+• °K
+• mg/L
+• ppm
+• ng/L
+• μg/L
+• cfu per mL
+• cfu per 100 ml</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">One of the following:
-• (blank), S/m, C, F, K, mg/L, ppm, ng/L, μg/L, cfu per mL, cfu per 100 ml.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One of the following:
-• Yield
+• Abstraction
 • Spring discharge</t>
   </si>
   <si>
@@ -99,6 +165,9 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">³/s
+• m³/m
+• m³/h
+• m³/d
 </t>
     </r>
     <r>
@@ -110,11 +179,15 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">• ft³/s</t>
+      <t xml:space="preserve">• ft³/s
+• ft³/m
+• ft³/h
+• ft³/d
+• L/s
+• L/m
+• L/h
+• L/d</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Explain the methodology used to collect the data</t>
   </si>
 </sst>
 </file>
@@ -349,7 +422,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="A1:F2 C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -424,7 +497,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="A1:F2 D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -462,16 +535,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>11</v>
@@ -499,7 +572,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -537,19 +610,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>

</xml_diff>